<commit_message>
Added test data for ignore flight for invoicing
</commit_message>
<xml_diff>
--- a/src/FLS.Server.Tests/TestData/FlightInvoiceTestdata.xlsx
+++ b/src/FLS.Server.Tests/TestData/FlightInvoiceTestdata.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="260">
   <si>
     <t>UseCase</t>
   </si>
@@ -902,6 +902,18 @@
   <si>
     <t>Rechnung mit 1 Position an Piloten: _x000D_
 1. Startgebühr Eigenstarter</t>
+  </si>
+  <si>
+    <t>Privater Flug ab Schänis nach Schänis</t>
+  </si>
+  <si>
+    <t>Privatflug extern --&gt; keine Verrechnung</t>
+  </si>
+  <si>
+    <t>Für Privatflugzeuge auf externen Flugplätzen soll keine Rechnung erstellt werden.</t>
+  </si>
+  <si>
+    <t>Keine Rechnung</t>
   </si>
 </sst>
 </file>
@@ -1729,10 +1741,10 @@
   <dimension ref="A1:BL41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E39" sqref="E39"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6760,6 +6772,65 @@
         <v>252</v>
       </c>
     </row>
+    <row r="40" spans="1:46" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>35</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="J40" s="1">
+        <v>3</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="P40" s="1">
+        <v>61</v>
+      </c>
+      <c r="Q40" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="R40" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="S40" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="T40" s="1">
+        <v>200</v>
+      </c>
+      <c r="U40">
+        <v>500</v>
+      </c>
+      <c r="V40" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="AC40" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD40" s="1">
+        <v>0</v>
+      </c>
+    </row>
     <row r="41" spans="1:46" x14ac:dyDescent="0.25">
       <c r="H41" s="4"/>
     </row>

</xml_diff>